<commit_message>
fixed contour, expanded plotCEA, added to main, minor bug fixes
</commit_message>
<xml_diff>
--- a/input/250lbf.xlsx
+++ b/input/250lbf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shortcuts\Documents\GitHub\engine-sizing\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E7F716-D73A-4786-BC22-02AF66BE2764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6526FD-A876-4DAC-B0B8-F9D47AF0DC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
     <definedName name="y" localSheetId="2">Injector!#REF!</definedName>
     <definedName name="y">Definition!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateCount="1000"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -147,7 +147,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="158">
   <si>
     <t>Run Description:</t>
   </si>
@@ -782,13 +782,7 @@
     </r>
   </si>
   <si>
-    <t>crude</t>
-  </si>
-  <si>
     <t>diameter</t>
-  </si>
-  <si>
-    <t>throat</t>
   </si>
   <si>
     <t>whether or not to size engine (boolean)</t>
@@ -887,6 +881,18 @@
   </si>
   <si>
     <t>options: "impinging", "pintle", "swirl", "shear"</t>
+  </si>
+  <si>
+    <t>C3H8O,1propanol</t>
+  </si>
+  <si>
+    <t>Isopropyl Alcohol (IPA)</t>
+  </si>
+  <si>
+    <t>throat</t>
+  </si>
+  <si>
+    <t>bell</t>
   </si>
 </sst>
 </file>
@@ -1239,7 +1245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1328,6 +1334,9 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1767,23 +1776,23 @@
     <col min="6" max="16384" width="9.140625" style="40"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="44" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:8" s="45" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-    </row>
-    <row r="3" spans="1:8" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
+    <row r="2" spans="1:8" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="46"/>
+    </row>
+    <row r="3" spans="1:8" s="49" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="48"/>
     </row>
     <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="50"/>
+      <c r="C5" s="51"/>
     </row>
     <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26" t="s">
@@ -1808,47 +1817,47 @@
       </c>
       <c r="C10" s="38"/>
       <c r="D10" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E10" s="16"/>
     </row>
     <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E11" s="16"/>
     </row>
     <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C12" s="38"/>
       <c r="D12" s="24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C13" s="38"/>
       <c r="D13" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C14" s="38"/>
       <c r="D14" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -1856,58 +1865,58 @@
     </row>
     <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C16" s="39"/>
       <c r="D16" s="20"/>
     </row>
     <row r="17" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C17" s="34"/>
       <c r="D17" s="24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C18" s="34"/>
       <c r="D18" s="24" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C19" s="34"/>
       <c r="D19" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C20" s="34"/>
       <c r="D20" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="51" t="s">
-        <v>153</v>
-      </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
+      <c r="B22" s="52" t="s">
+        <v>151</v>
+      </c>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
     </row>
     <row r="23" spans="2:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
+      <c r="B23" s="52"/>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1922,10 +1931,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3FB38BB-BE64-4050-8878-0E451113B9D1}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32:J32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1936,7 +1945,7 @@
     <col min="4" max="4" width="7" style="12" customWidth="1"/>
     <col min="5" max="5" width="41" style="17" customWidth="1"/>
     <col min="6" max="6" width="4.7109375" style="12" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="12" customWidth="1"/>
     <col min="8" max="8" width="11" style="12" customWidth="1"/>
     <col min="9" max="9" width="7.140625" style="12" customWidth="1"/>
     <col min="10" max="10" width="45" style="16" customWidth="1"/>
@@ -1948,24 +1957,24 @@
     <col min="16" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="53" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:15" s="54" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="53" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="55" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54"/>
-    </row>
-    <row r="3" spans="1:15" s="57" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="56"/>
+    <row r="2" spans="1:15" s="56" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="55"/>
+    </row>
+    <row r="3" spans="1:15" s="58" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="57"/>
     </row>
     <row r="4" spans="1:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:15" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="60"/>
-      <c r="D5" s="61"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="62"/>
       <c r="E5" s="16"/>
     </row>
     <row r="7" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2030,7 +2039,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="33">
-        <v>14.7</v>
+        <v>11</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>22</v>
@@ -2042,7 +2051,7 @@
         <v>37</v>
       </c>
       <c r="H10" s="33" t="s">
-        <v>66</v>
+        <v>154</v>
       </c>
       <c r="I10" s="13"/>
       <c r="J10" s="24" t="s">
@@ -2052,7 +2061,7 @@
         <v>44</v>
       </c>
       <c r="M10" s="34" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="N10" s="13"/>
       <c r="O10" s="5" t="s">
@@ -2084,7 +2093,7 @@
         <v>31</v>
       </c>
       <c r="M11" s="34" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
       <c r="N11" s="13"/>
       <c r="O11" s="5" t="s">
@@ -2116,11 +2125,11 @@
         <v>96</v>
       </c>
       <c r="M12" s="34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N12" s="13"/>
       <c r="O12" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2128,7 +2137,7 @@
         <v>34</v>
       </c>
       <c r="C13" s="34">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>11</v>
@@ -2165,7 +2174,7 @@
         <v>43</v>
       </c>
       <c r="H14" s="33">
-        <v>2.1</v>
+        <v>1.3</v>
       </c>
       <c r="I14" s="13"/>
       <c r="J14" s="24" t="s">
@@ -2183,7 +2192,7 @@
         <v>45</v>
       </c>
       <c r="M15" s="34">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="N15" s="13" t="s">
         <v>13</v>
@@ -2193,12 +2202,12 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="64" t="s">
+      <c r="B16" s="65" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="64"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
       <c r="G16" s="19" t="s">
         <v>60</v>
       </c>
@@ -2209,7 +2218,7 @@
         <v>122</v>
       </c>
       <c r="M16" s="34">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="N16" s="13" t="s">
         <v>17</v>
@@ -2219,10 +2228,10 @@
       </c>
     </row>
     <row r="17" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="64"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="64"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="65"/>
+      <c r="D17" s="65"/>
+      <c r="E17" s="65"/>
       <c r="G17" s="13" t="s">
         <v>123</v>
       </c>
@@ -2261,7 +2270,7 @@
         <v>120</v>
       </c>
       <c r="M18" s="37">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="N18" s="13" t="s">
         <v>13</v>
@@ -2275,7 +2284,7 @@
         <v>121</v>
       </c>
       <c r="M19" s="37">
-        <v>0.875</v>
+        <v>0.75</v>
       </c>
       <c r="N19" s="13" t="s">
         <v>13</v>
@@ -2285,18 +2294,18 @@
       </c>
     </row>
     <row r="20" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G20" s="64" t="s">
+      <c r="G20" s="65" t="s">
         <v>114</v>
       </c>
-      <c r="H20" s="64"/>
-      <c r="I20" s="64"/>
-      <c r="J20" s="64"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
     </row>
     <row r="21" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
       <c r="L21" s="19" t="s">
         <v>53</v>
       </c>
@@ -2315,7 +2324,7 @@
         <v>11</v>
       </c>
       <c r="O22" s="24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2328,12 +2337,12 @@
       <c r="M23" s="35"/>
     </row>
     <row r="24" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G24" s="66" t="s">
+      <c r="G24" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="66"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
       <c r="L24" s="19" t="s">
         <v>52</v>
       </c>
@@ -2343,10 +2352,10 @@
     </row>
     <row r="25" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C25" s="22"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="62"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="63"/>
       <c r="L25" s="13" t="s">
         <v>115</v>
       </c>
@@ -2361,10 +2370,10 @@
       </c>
     </row>
     <row r="26" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
       <c r="L26" s="25" t="s">
         <v>116</v>
       </c>
@@ -2403,197 +2412,207 @@
       <c r="G28" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H28" s="67" t="s">
+      <c r="H28" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="I28" s="67"/>
-      <c r="J28" s="67"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
     </row>
     <row r="29" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G29" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="H29" s="65" t="s">
+      <c r="H29" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="I29" s="65"/>
-      <c r="J29" s="65"/>
-      <c r="L29" s="64" t="s">
+      <c r="I29" s="66"/>
+      <c r="J29" s="66"/>
+      <c r="L29" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="M29" s="64"/>
-      <c r="N29" s="64"/>
-      <c r="O29" s="64"/>
+      <c r="M29" s="65"/>
+      <c r="N29" s="65"/>
+      <c r="O29" s="65"/>
     </row>
     <row r="30" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G30" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="H30" s="65" t="s">
+      <c r="H30" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="I30" s="65"/>
-      <c r="J30" s="65"/>
-      <c r="L30" s="64"/>
-      <c r="M30" s="64"/>
-      <c r="N30" s="64"/>
-      <c r="O30" s="64"/>
+      <c r="I30" s="66"/>
+      <c r="J30" s="66"/>
+      <c r="L30" s="65"/>
+      <c r="M30" s="65"/>
+      <c r="N30" s="65"/>
+      <c r="O30" s="65"/>
     </row>
     <row r="31" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G31" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H31" s="65" t="s">
+      <c r="H31" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="I31" s="65"/>
-      <c r="J31" s="65"/>
+      <c r="I31" s="66"/>
+      <c r="J31" s="66"/>
     </row>
     <row r="32" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G32" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H32" s="65" t="s">
+      <c r="H32" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="I32" s="65"/>
-      <c r="J32" s="65"/>
-      <c r="L32" s="64" t="s">
-        <v>147</v>
-      </c>
-      <c r="M32" s="64"/>
-      <c r="N32" s="64"/>
-      <c r="O32" s="64"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="66"/>
+      <c r="L32" s="65" t="s">
+        <v>145</v>
+      </c>
+      <c r="M32" s="65"/>
+      <c r="N32" s="65"/>
+      <c r="O32" s="65"/>
     </row>
     <row r="33" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G33" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="65" t="s">
+      <c r="H33" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="I33" s="65"/>
-      <c r="J33" s="65"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
-      <c r="N33" s="64"/>
-      <c r="O33" s="64"/>
+      <c r="I33" s="66"/>
+      <c r="J33" s="66"/>
+      <c r="L33" s="65"/>
+      <c r="M33" s="65"/>
+      <c r="N33" s="65"/>
+      <c r="O33" s="65"/>
     </row>
     <row r="34" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G34" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="H34" s="65" t="s">
+      <c r="H34" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="I34" s="65"/>
-      <c r="J34" s="65"/>
+      <c r="I34" s="66"/>
+      <c r="J34" s="66"/>
       <c r="L34" s="14"/>
       <c r="M34" s="14"/>
       <c r="N34" s="14"/>
       <c r="O34" s="14"/>
     </row>
     <row r="35" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="L35" s="64"/>
-      <c r="M35" s="64"/>
-      <c r="N35" s="64"/>
-      <c r="O35" s="64"/>
+      <c r="G35" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="I35" s="13"/>
+      <c r="J35" s="24"/>
+      <c r="L35" s="65"/>
+      <c r="M35" s="65"/>
+      <c r="N35" s="65"/>
+      <c r="O35" s="65"/>
     </row>
     <row r="36" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G36" s="19" t="s">
+      <c r="L36" s="65"/>
+      <c r="M36" s="65"/>
+      <c r="N36" s="65"/>
+      <c r="O36" s="65"/>
+    </row>
+    <row r="37" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G37" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="21"/>
-      <c r="L36" s="64"/>
-      <c r="M36" s="64"/>
-      <c r="N36" s="64"/>
-      <c r="O36" s="64"/>
-    </row>
-    <row r="37" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G37" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H37" s="67" t="s">
-        <v>83</v>
-      </c>
-      <c r="I37" s="67"/>
-      <c r="J37" s="67"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="21"/>
       <c r="L37" s="14"/>
       <c r="M37" s="14"/>
       <c r="N37" s="14"/>
       <c r="O37" s="14"/>
     </row>
     <row r="38" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="62" t="s">
+      <c r="B38" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="C38" s="62"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="62"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="63"/>
+      <c r="E38" s="63"/>
       <c r="G38" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H38" s="68" t="s">
+        <v>83</v>
+      </c>
+      <c r="I38" s="68"/>
+      <c r="J38" s="68"/>
+    </row>
+    <row r="39" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="64"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="G39" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="H38" s="65" t="s">
+      <c r="H39" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="I38" s="65"/>
-      <c r="J38" s="65"/>
-    </row>
-    <row r="39" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="63"/>
-      <c r="C39" s="63"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="63"/>
-      <c r="G39" s="13" t="s">
+      <c r="I39" s="66"/>
+      <c r="J39" s="66"/>
+    </row>
+    <row r="40" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="64"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+      <c r="G40" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="H39" s="65" t="s">
+      <c r="H40" s="66" t="s">
         <v>85</v>
       </c>
-      <c r="I39" s="65"/>
-      <c r="J39" s="65"/>
-    </row>
-    <row r="40" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="63"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="63"/>
-      <c r="G40" s="13" t="s">
+      <c r="I40" s="66"/>
+      <c r="J40" s="66"/>
+    </row>
+    <row r="41" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G41" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="H40" s="65" t="s">
+      <c r="H41" s="66" t="s">
         <v>86</v>
       </c>
-      <c r="I40" s="65"/>
-      <c r="J40" s="65"/>
-    </row>
-    <row r="43" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G43" s="58"/>
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
-      <c r="J43" s="58"/>
+      <c r="I41" s="66"/>
+      <c r="J41" s="66"/>
     </row>
     <row r="44" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G44" s="58"/>
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
-      <c r="J44" s="58"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
+    </row>
+    <row r="45" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="H33:J33"/>
     <mergeCell ref="H34:J34"/>
-    <mergeCell ref="H37:J37"/>
     <mergeCell ref="H38:J38"/>
     <mergeCell ref="H39:J39"/>
+    <mergeCell ref="H40:J40"/>
     <mergeCell ref="A1:XFD3"/>
-    <mergeCell ref="G43:J44"/>
+    <mergeCell ref="G44:J45"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B38:E40"/>
     <mergeCell ref="B16:E17"/>
-    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="H41:J41"/>
     <mergeCell ref="L35:O36"/>
     <mergeCell ref="G24:J26"/>
     <mergeCell ref="G20:J21"/>
@@ -2615,7 +2634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2558753-C1A4-4F1A-A391-5DC27086ECDF}">
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -2639,23 +2658,23 @@
     <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="44" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+    <row r="1" spans="1:10" s="45" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="46" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-    </row>
-    <row r="3" spans="1:10" s="48" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
+    <row r="2" spans="1:10" s="47" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="46"/>
+    </row>
+    <row r="3" spans="1:10" s="49" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="48"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:10" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="50"/>
+      <c r="C5" s="51"/>
       <c r="E5" s="8" t="s">
         <v>19</v>
       </c>
@@ -2743,7 +2762,7 @@
         <v>13</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>